<commit_message>
Page Factories - Implementing Parameterization and Runmodes to the test case
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark\Documents\IntelliJ\Udemy\Architect\PageObjectModelBasics\src\test\resources\com\w2a\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark\Documents\IntelliJ\Udemy\Architect\PageObjectwithFactories\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{905037CF-FD40-4FA5-A464-6C67740F7CA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{145F4EE4-CD12-4121-9E63-D3CF7BBC6427}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="test_suite" sheetId="3" r:id="rId1"/>
-    <sheet name="LoginTest" sheetId="1" r:id="rId2"/>
-    <sheet name="createAccountTest" sheetId="4" r:id="rId3"/>
+    <sheet name="signInTest" sheetId="1" r:id="rId1"/>
+    <sheet name="flightSearchTest" sheetId="5" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,26 +34,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
-  <si>
-    <t>Raman</t>
-  </si>
-  <si>
-    <t>TCID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>Y</t>
   </si>
   <si>
-    <t>Runmode</t>
-  </si>
-  <si>
     <t>runmode</t>
   </si>
   <si>
-    <t>LoginTest</t>
-  </si>
-  <si>
     <t>username</t>
   </si>
   <si>
@@ -67,10 +54,34 @@
     <t>Selenium@123</t>
   </si>
   <si>
-    <t>CreateAccountTest</t>
-  </si>
-  <si>
-    <t>accountname</t>
+    <t>java@gmail.com</t>
+  </si>
+  <si>
+    <t>fromCity</t>
+  </si>
+  <si>
+    <t>toCity</t>
+  </si>
+  <si>
+    <t>Vienna</t>
+  </si>
+  <si>
+    <t>Berlin</t>
+  </si>
+  <si>
+    <t>fromDate</t>
+  </si>
+  <si>
+    <t>toDate</t>
+  </si>
+  <si>
+    <t>13/07/2020</t>
+  </si>
+  <si>
+    <t>20/07/2020</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -115,9 +126,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -460,54 +472,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEDB6888-7696-4AF5-B1FE-58A9156BB586}">
-  <dimension ref="A1:B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,57 +487,88 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{1DC5759E-7B06-42E6-9AE6-9728F815A879}"/>
     <hyperlink ref="B2" r:id="rId2" xr:uid="{4BE6A518-4E6E-43F7-A281-2BA42961CD18}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{66315BEA-88B1-4F4F-B3E4-3B164942D1C3}"/>
+    <hyperlink ref="B3" r:id="rId4" xr:uid="{89D7D66F-1786-4829-BB00-4253F9724588}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAC343F5-901A-45D0-B097-EE83E29D70AB}">
-  <dimension ref="A1:A2"/>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2D037DB-29D8-4957-8515-DF760D40B7FC}">
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>